<commit_message>
Updated variable defintions document
</commit_message>
<xml_diff>
--- a/Extra/ActiPASS_Variable-definitions_NewFormat_20220517.xlsx
+++ b/Extra/ActiPASS_Variable-definitions_NewFormat_20220517.xlsx
@@ -5,22 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Bronze\Ergonomiforsk\ActiPASS\Documentation\Variable Dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pashe866\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionary" sheetId="1" r:id="rId1"/>
-    <sheet name="Appendix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="197">
   <si>
     <t>varNames</t>
   </si>
@@ -353,36 +352,6 @@
     <t>Only available when work/leisure diary is given</t>
   </si>
   <si>
-    <t>SED_1</t>
-  </si>
-  <si>
-    <t>LPA_1</t>
-  </si>
-  <si>
-    <t>MPA_1</t>
-  </si>
-  <si>
-    <t>MVPA_1</t>
-  </si>
-  <si>
-    <t>VPA_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time spent on activities classified as sedentary </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time spent on activities classified as low-physical activity </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time spent on activities classified as moderate physical activity </t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as vigorous  physical activity</t>
-  </si>
-  <si>
-    <t>Time spent on activities classified as moderate or  vigorous  physical activity</t>
-  </si>
-  <si>
     <t>Important Note: These variables are calculated using the direct output of activity detection algorithm with an epoch of 1s. Any sporadic break, misclassification or ambiguity can affect these variables. These variables, except for the combined activity/posture "SitLie", should only be used with consultation of ActiPASS developers</t>
   </si>
   <si>
@@ -492,9 +461,6 @@
     <t>replace "SitLie" with the relevant activity/posture/intensity-class to derive corresponding variable name (also see notice above)</t>
   </si>
   <si>
-    <t>Time spent on different energy expenditure intensity classes. See the separate appendix for how intensity classes are derived. All times are given in minutes</t>
-  </si>
-  <si>
     <t>A day can be further sub-divided into domains such as 'Work' and 'Leisure' and following variables can be generated for each such sub-domain within a calendar day.  Such variables will be prefixed with the domain (Ex. Work_Duration_1) This additional domain specific data is available only when the additional diary containing such data is included in ActiPASS processing, and also the relevant domain names are specified under "Stat Domains" options before stats generation.</t>
   </si>
   <si>
@@ -506,55 +472,73 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">Activity/Posture times and cadence related variables. These variables are defined within "Awake". All times are given in minutes. These variables satisfy the equation:  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Awake=Lie+Sit+Stand+Move+Walk+Run+Stair+Cycle+Other</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t>Variables related to the bedtime, sleep-interval and awake time. All times are given in minutes. These variables satisfy the equation:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ValidDuration = Awake + SleepInterval</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">The posture </t>
+      <t xml:space="preserve">Variables related to exclusions, non-wear and validity. All times are given in minutes. These variables satisfy the equations: </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>"SitLie"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -570,11 +554,9 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, SED, LPA, MPA, VPA, MVPA
+      <t xml:space="preserve">Duration = Excluded + NonWear + ValidDuration
 </t>
     </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -583,69 +565,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Activity/Posture times and cadence related variables. These variables are defined within "Awake". All times are given in minutes. These variables satisfy the equation:  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">                      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Awake=Lie+Sit+Stand+Move+Walk+Run+Stair+Cycle+Other</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Variables related to the bedtime, sleep-interval and awake time. All times are given in minutes. These variables satisfy the equation:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ValidDuration = Awake + SleepInterval</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="5" tint="-0.499984740745262"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Variables related to exclusions, non-wear and validity. All times are given in minutes. These variables satisfy the equations: </t>
+      <t>and</t>
     </r>
     <r>
       <rPr>
@@ -665,22 +585,271 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Duration = Excluded + NonWear + ValidDuration
+      <t xml:space="preserve">NonWear = AwakeNW +  SlpIntNW
 </t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The time of NW </t>
+    </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>outside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The time of NW </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>inside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
+    </r>
+  </si>
+  <si>
+    <t>SitLie_1min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_bouts_TH_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_freq_H_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_bouts_TL_1</t>
+  </si>
+  <si>
+    <t>SitLie_1min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_2min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_3min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_4min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_5min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_10min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_30min_freq_L_1</t>
+  </si>
+  <si>
+    <t>SitLie_60min_freq_L_1</t>
+  </si>
+  <si>
+    <t> Intensity class name</t>
+  </si>
+  <si>
+    <t>INT1_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as sedentary on day 1</t>
+  </si>
+  <si>
+    <t>INT2_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as low physical activity on day 1</t>
+  </si>
+  <si>
+    <t>INT2_Amb_1</t>
+  </si>
+  <si>
+    <t>Time spent on ambulatory activities classified as low physical activity  (standing excluded) on day 1</t>
+  </si>
+  <si>
+    <t>INT3_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as moderate physical activity on day 1</t>
+  </si>
+  <si>
+    <t> How times are derived</t>
+  </si>
+  <si>
+    <t>"Sit" and "Lie"</t>
+  </si>
+  <si>
+    <t>"Stand", "Move", "Walk_Slow" (walking with a cadence lower than 100/min), and "Other" with no periodic movements and "Other" with periodic movements with a cadence lower than 100/min)</t>
+  </si>
+  <si>
+    <t>"Move", "Walk_Slow" (walking with a cadence lower than 100/min), "Other" with no periodic movements, and "Other" with periodic movements with a cadence lower than 100/min)</t>
+  </si>
+  <si>
+    <t>"Walk" (with a cadence between 100-130/min) and "Other" with periodic movements with a cadence between 100-130/min</t>
+  </si>
+  <si>
+    <t>INT4_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as vigorous  physical activity on day 1</t>
+  </si>
+  <si>
+    <t>"Run", "Cycle", "Stair", "Walk" with a cadence higher than 130/min , "Other" with periodic movement with a cadence higher than or equal to 130/min</t>
+  </si>
+  <si>
+    <t>INT34_1</t>
+  </si>
+  <si>
+    <t>Time spent on activities classified as moderate and vigorous  physical activity on day 1</t>
+  </si>
+  <si>
+    <t>"INT3" and "INT4"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time spent on different energy expenditure intensity classes </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
         <color theme="5" tint="-0.499984740745262"/>
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>and</t>
+      <t>Time percentiles of continuous segments of activity/posture/intensity-classes  and breaks of activity/posture/intensity-classes.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">The posture </t>
     </r>
     <r>
       <rPr>
         <b/>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>"SitLie"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.499984740745262"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> is chosen as an example. These Variables are also derived for following activity/postures as well as intensity classes.</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -696,52 +865,8 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">NonWear = AwakeNW +  SlpIntNW
+      <t xml:space="preserve">Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, INT1, INT2, INT2_Amb, INT3, INT4, INT34
 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The time of NW </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>outside</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The time of NW </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>inside</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> any periods flagged as sleep-intervals. There could be more than one sleep-intervals happening for a given calendar day</t>
     </r>
   </si>
   <si>
@@ -773,170 +898,8 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other, SED, LPA, MPA, VPA, MVPA</t>
-    </r>
-  </si>
-  <si>
-    <t>Settings.MET_SI=0.95;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Lie=1.0;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Sit=1.3;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Stand=1.4;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Move=2.0;</t>
-  </si>
-  <si>
-    <t>Settings.Wlk_Low_MET=2;</t>
-  </si>
-  <si>
-    <t>Settings.Wlk_Fast_MET=4;</t>
-  </si>
-  <si>
-    <t>Settings.Wlk_VFast_MET=7;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Running=10;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Stairs=8;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Cycle=7;</t>
-  </si>
-  <si>
-    <t>Settings.MET_Other=2;</t>
-  </si>
-  <si>
-    <t>% MET citoffs for intensity classes</t>
-  </si>
-  <si>
-    <t>%Settings.PA_Slp=0.0;</t>
-  </si>
-  <si>
-    <t>Settings.PA_SED=1.0;</t>
-  </si>
-  <si>
-    <t>Settings.PA_LPA=1.5;</t>
-  </si>
-  <si>
-    <t>Settings.PA_MPA=3.0;</t>
-  </si>
-  <si>
-    <t>Settings.PA_VPA=6.0;</t>
-  </si>
-  <si>
-    <t>%cadence cutoffs for walk-slow, walk-fast and walk-very-fast</t>
-  </si>
-  <si>
-    <t>Settings.Wlk_Slow_Cad=100;</t>
-  </si>
-  <si>
-    <t>Settings.Wlk_VFast_Cad=130;</t>
-  </si>
-  <si>
-    <t>Aactivity/posture to equivalent MET translation</t>
-  </si>
-  <si>
-    <t>SitLie_1min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_bouts_TH_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_freq_H_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_bouts_TL_1</t>
-  </si>
-  <si>
-    <t>SitLie_1min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_2min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_3min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_4min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_5min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_10min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_30min_freq_L_1</t>
-  </si>
-  <si>
-    <t>SitLie_60min_freq_L_1</t>
+      <t>Lie, Sit, SitLie, Stand, Move, StandMove,  Walk, Run, Stair, Cycle, Other,INT1, INT2, INT2_Amb, INT3, INT4, INT34</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1029,11 +992,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF833C0C"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1062,11 +1025,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1131,16 +1095,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -1173,8 +1160,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1205,10 +1190,21 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1219,11 +1215,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="40% - Accent5" xfId="4" builtinId="47"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
@@ -1503,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C107"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1596,11 +1591,11 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" s="21" customFormat="1" ht="60">
-      <c r="B10" s="23" t="s">
+    <row r="10" spans="1:3" s="19" customFormat="1" ht="60">
+      <c r="B10" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="22"/>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
@@ -1660,19 +1655,19 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" s="17" customFormat="1" ht="90">
-      <c r="B18" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="18"/>
-    </row>
-    <row r="19" spans="1:3" s="17" customFormat="1">
-      <c r="B19" s="19"/>
-      <c r="C19" s="18"/>
+    <row r="18" spans="1:3" s="15" customFormat="1" ht="90">
+      <c r="B18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:3" s="15" customFormat="1">
+      <c r="B19" s="17"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" s="5" customFormat="1" ht="91.5" customHeight="1">
-      <c r="B20" s="26" t="s">
-        <v>151</v>
+      <c r="B20" s="24" t="s">
+        <v>139</v>
       </c>
       <c r="C20" s="6"/>
     </row>
@@ -1708,7 +1703,7 @@
         <v>92</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -1717,7 +1712,7 @@
         <v>93</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C25" s="4"/>
     </row>
@@ -1731,8 +1726,8 @@
       <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" s="5" customFormat="1" ht="48.75" customHeight="1">
-      <c r="B27" s="26" t="s">
-        <v>150</v>
+      <c r="B27" s="24" t="s">
+        <v>138</v>
       </c>
       <c r="C27" s="6"/>
     </row>
@@ -1781,8 +1776,8 @@
       </c>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1" ht="54.75" customHeight="1">
-      <c r="B33" s="26" t="s">
-        <v>149</v>
+      <c r="B33" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="C33" s="6"/>
     </row>
@@ -1902,597 +1897,511 @@
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="1:3" s="5" customFormat="1"/>
-    <row r="48" spans="1:3" s="5" customFormat="1" ht="30">
-      <c r="B48" s="25" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>105</v>
+    <row r="48" spans="1:3" s="5" customFormat="1">
+      <c r="B48" s="23" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A49" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" s="5" customFormat="1"/>
+      <c r="A50" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="45">
+      <c r="A51" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="45">
+      <c r="A52" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="30">
+      <c r="A53" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30">
+      <c r="A54" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="5" customFormat="1">
+      <c r="A55" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>193</v>
+      </c>
+    </row>
     <row r="56" spans="1:3" s="5" customFormat="1">
-      <c r="B56" s="24" t="s">
+      <c r="A56" s="28"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+    </row>
+    <row r="57" spans="1:3" s="5" customFormat="1">
+      <c r="B57" s="22" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>26</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B60" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="5" customFormat="1" ht="120">
-      <c r="B62" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C62" s="16" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="C63" s="30" t="s">
-        <v>111</v>
+    <row r="63" spans="1:3" s="5" customFormat="1" ht="120">
+      <c r="B63" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>31</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C64" s="31"/>
+      <c r="C64" s="31" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C65" s="31"/>
+        <v>76</v>
+      </c>
+      <c r="C65" s="32"/>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C66" s="31"/>
+        <v>71</v>
+      </c>
+      <c r="C66" s="32"/>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C67" s="31"/>
+        <v>72</v>
+      </c>
+      <c r="C67" s="32"/>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>35</v>
-      </c>
-      <c r="B68" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C68" s="31"/>
+        <v>34</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C68" s="32"/>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C69" s="31"/>
+        <v>77</v>
+      </c>
+      <c r="C69" s="32"/>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="32"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C70" s="31"/>
-    </row>
-    <row r="71" spans="1:3" ht="30">
-      <c r="A71" t="s">
+      <c r="C71" s="32"/>
+    </row>
+    <row r="72" spans="1:3" ht="30">
+      <c r="A72" t="s">
         <v>38</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="31"/>
-    </row>
-    <row r="74" spans="1:3" s="5" customFormat="1" ht="90">
-      <c r="B74" s="26" t="s">
-        <v>154</v>
-      </c>
-      <c r="C74" s="27" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>177</v>
-      </c>
-      <c r="B76" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C76" s="32" t="s">
-        <v>145</v>
+      <c r="C72" s="32"/>
+    </row>
+    <row r="75" spans="1:3" s="5" customFormat="1" ht="90">
+      <c r="B75" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C75" s="25" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C77" s="32"/>
+        <v>103</v>
+      </c>
+      <c r="C77" s="33" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="C78" s="32"/>
+        <v>104</v>
+      </c>
+      <c r="C78" s="33"/>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="C79" s="32"/>
+        <v>105</v>
+      </c>
+      <c r="C79" s="33"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C80" s="32"/>
+        <v>106</v>
+      </c>
+      <c r="C80" s="33"/>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="C81" s="32"/>
+        <v>107</v>
+      </c>
+      <c r="C81" s="33"/>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C82" s="32"/>
+        <v>108</v>
+      </c>
+      <c r="C82" s="33"/>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C83" s="32"/>
+        <v>109</v>
+      </c>
+      <c r="C83" s="33"/>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>192</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C84" s="32"/>
+        <v>149</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C84" s="33"/>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C85" s="32"/>
+        <v>111</v>
+      </c>
+      <c r="C85" s="33"/>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C86" s="32"/>
+        <v>112</v>
+      </c>
+      <c r="C86" s="33"/>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C87" s="32"/>
+        <v>113</v>
+      </c>
+      <c r="C87" s="33"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="C88" s="32"/>
+        <v>114</v>
+      </c>
+      <c r="C88" s="33"/>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C89" s="32"/>
+        <v>115</v>
+      </c>
+      <c r="C89" s="33"/>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C90" s="32"/>
+        <v>116</v>
+      </c>
+      <c r="C90" s="33"/>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C91" s="32"/>
+        <v>117</v>
+      </c>
+      <c r="C91" s="33"/>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>193</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C92" s="32"/>
+        <v>156</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C92" s="33"/>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C93" s="32"/>
+        <v>119</v>
+      </c>
+      <c r="C93" s="33"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C94" s="32"/>
+        <v>120</v>
+      </c>
+      <c r="C94" s="33"/>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C95" s="32"/>
+        <v>121</v>
+      </c>
+      <c r="C95" s="33"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C96" s="32"/>
+        <v>122</v>
+      </c>
+      <c r="C96" s="33"/>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C97" s="32"/>
+        <v>123</v>
+      </c>
+      <c r="C97" s="33"/>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="B98" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C98" s="32"/>
+        <v>124</v>
+      </c>
+      <c r="C98" s="33"/>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C99" s="32"/>
+        <v>125</v>
+      </c>
+      <c r="C99" s="33"/>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>201</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="C100" s="32"/>
+        <v>165</v>
+      </c>
+      <c r="B100" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C100" s="33"/>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C101" s="32"/>
+        <v>134</v>
+      </c>
+      <c r="C101" s="33"/>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C102" s="32"/>
+        <v>127</v>
+      </c>
+      <c r="C102" s="33"/>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C103" s="32"/>
+        <v>128</v>
+      </c>
+      <c r="C103" s="33"/>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C104" s="32"/>
+        <v>129</v>
+      </c>
+      <c r="C104" s="33"/>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C105" s="32"/>
+        <v>130</v>
+      </c>
+      <c r="C105" s="33"/>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C106" s="32"/>
+        <v>131</v>
+      </c>
+      <c r="C106" s="33"/>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C107" s="32"/>
+        <v>132</v>
+      </c>
+      <c r="C107" s="33"/>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>173</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C108" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C63:C71"/>
-    <mergeCell ref="C76:C107"/>
+    <mergeCell ref="C64:C72"/>
+    <mergeCell ref="C77:C108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:A26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="52.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:1" s="29" customFormat="1">
-      <c r="A3" s="28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" s="29" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A17" s="29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="14" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" s="29" customFormat="1">
-      <c r="A24" s="29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>175</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>